<commit_message>
Data fix for flat plate
</commit_message>
<xml_diff>
--- a/Student Version Summer 25/Design Input Files/Design Input File_V25-00-WingAR.xlsx
+++ b/Student Version Summer 25/Design Input Files/Design Input File_V25-00-WingAR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thekl\Documents\MATLAB\ASEN2804\ASEN2804_Su25_Lab1\Student Version Summer 25\Design Input Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natei\Documents\MATLAB\Summer 2025\ASEN 2804\Student Version Summer 25\Design Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DFBC18-A411-4115-A28D-678AB9445FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0D1DCB-E4DA-47D2-8AD7-90A47A078D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="2085" windowWidth="14400" windowHeight="8183" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -3520,10 +3520,10 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.9" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.5546875" customWidth="1"/>
+    <col min="2" max="4" width="30.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50.1" customHeight="1">
@@ -3544,14 +3544,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15.6">
+    <row r="9" spans="2:4" ht="15.75">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" ht="15.6">
+    <row r="10" spans="2:4" ht="15.75">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -3560,14 +3560,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15.6">
+    <row r="11" spans="2:4" ht="15.75">
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="15.6">
+    <row r="12" spans="2:4" ht="15.75">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -3576,14 +3576,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15.6">
+    <row r="13" spans="2:4" ht="15.75">
       <c r="B13" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" ht="15.6">
+    <row r="14" spans="2:4" ht="15.75">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -3592,14 +3592,14 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15.6">
+    <row r="15" spans="2:4" ht="15.75">
       <c r="B15" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" ht="15.6">
+    <row r="16" spans="2:4" ht="15.75">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -3608,14 +3608,14 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15.6">
+    <row r="17" spans="2:4" ht="15.75">
       <c r="B17" s="2" t="s">
         <v>236</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" ht="15.6">
+    <row r="18" spans="2:4" ht="15.75">
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
         <v>5</v>
@@ -3624,14 +3624,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15.6">
+    <row r="19" spans="2:4" ht="15.75">
       <c r="B19" s="2" t="s">
         <v>245</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" ht="15.6">
+    <row r="20" spans="2:4" ht="15.75">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -3640,14 +3640,14 @@
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15.6">
+    <row r="21" spans="2:4" ht="15.75">
       <c r="B21" s="2" t="s">
         <v>249</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" ht="15.6">
+    <row r="22" spans="2:4" ht="15.75">
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
         <v>250</v>
@@ -3677,17 +3677,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A57" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="104.44140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="16.1328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.86328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="104.3984375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.265625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="8.86328125" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" customHeight="1">
@@ -3735,7 +3735,7 @@
       </c>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:5" ht="28.95" customHeight="1">
+    <row r="4" spans="1:5" ht="28.9" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="28.95" customHeight="1">
+    <row r="10" spans="1:5" ht="28.9" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -3855,7 +3855,7 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="28.95" customHeight="1">
+    <row r="12" spans="1:5" ht="28.9" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="28.95" customHeight="1">
+    <row r="14" spans="1:5" ht="28.9" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
@@ -3900,7 +3900,7 @@
       </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" ht="28.95" customHeight="1">
+    <row r="15" spans="1:5" ht="28.9" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>10</v>
       </c>
@@ -3975,7 +3975,7 @@
       </c>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" ht="43.2" customHeight="1">
+    <row r="20" spans="1:5" ht="43.15" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>10</v>
       </c>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5" ht="28.95" customHeight="1">
+    <row r="23" spans="1:5" ht="28.9" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>10</v>
       </c>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="E24" s="9"/>
     </row>
-    <row r="25" spans="1:5" ht="28.95" customHeight="1">
+    <row r="25" spans="1:5" ht="28.9" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>10</v>
       </c>
@@ -4080,7 +4080,7 @@
       </c>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="1:5" ht="28.95" customHeight="1">
+    <row r="27" spans="1:5" ht="28.9" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>10</v>
       </c>
@@ -4095,7 +4095,7 @@
       </c>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" ht="43.2" customHeight="1">
+    <row r="28" spans="1:5" ht="43.15" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>10</v>
       </c>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" ht="28.95" customHeight="1">
+    <row r="30" spans="1:5" ht="28.9" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>10</v>
       </c>
@@ -4140,7 +4140,7 @@
       </c>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="1:5" ht="28.95" customHeight="1">
+    <row r="31" spans="1:5" ht="28.9" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>10</v>
       </c>
@@ -4170,7 +4170,7 @@
       </c>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="1:5" ht="28.95" customHeight="1">
+    <row r="33" spans="1:5" ht="28.9" customHeight="1">
       <c r="A33" s="10" t="s">
         <v>10</v>
       </c>
@@ -4200,7 +4200,7 @@
       </c>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="1:5" ht="28.95" customHeight="1">
+    <row r="35" spans="1:5" ht="28.9" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>10</v>
       </c>
@@ -4215,7 +4215,7 @@
       </c>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="1:5" ht="43.2" customHeight="1">
+    <row r="36" spans="1:5" ht="43.15" customHeight="1">
       <c r="A36" s="10" t="s">
         <v>10</v>
       </c>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="E37" s="9"/>
     </row>
-    <row r="38" spans="1:5" ht="28.95" customHeight="1">
+    <row r="38" spans="1:5" ht="28.9" customHeight="1">
       <c r="A38" s="10" t="s">
         <v>10</v>
       </c>
@@ -4260,7 +4260,7 @@
       </c>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="1:5" ht="28.95" customHeight="1">
+    <row r="39" spans="1:5" ht="28.9" customHeight="1">
       <c r="A39" s="10" t="s">
         <v>10</v>
       </c>
@@ -4290,7 +4290,7 @@
       </c>
       <c r="E40" s="9"/>
     </row>
-    <row r="41" spans="1:5" ht="28.95" customHeight="1">
+    <row r="41" spans="1:5" ht="28.9" customHeight="1">
       <c r="A41" s="10" t="s">
         <v>10</v>
       </c>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="1:5" ht="28.95" customHeight="1">
+    <row r="43" spans="1:5" ht="28.9" customHeight="1">
       <c r="A43" s="10" t="s">
         <v>10</v>
       </c>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:5" ht="43.2" customHeight="1">
+    <row r="44" spans="1:5" ht="43.15" customHeight="1">
       <c r="A44" s="10" t="s">
         <v>10</v>
       </c>
@@ -4425,7 +4425,7 @@
       </c>
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="1:5" ht="28.95" customHeight="1">
+    <row r="50" spans="1:5" ht="28.9" customHeight="1">
       <c r="A50" s="10" t="s">
         <v>10</v>
       </c>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="1:5" ht="28.95" customHeight="1">
+    <row r="75" spans="1:5" ht="28.9" customHeight="1">
       <c r="A75" s="10" t="s">
         <v>149</v>
       </c>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="1:5" ht="28.95" customHeight="1">
+    <row r="78" spans="1:5" ht="28.9" customHeight="1">
       <c r="A78" s="10" t="s">
         <v>149</v>
       </c>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="E80" s="9"/>
     </row>
-    <row r="81" spans="1:5" ht="28.95" customHeight="1">
+    <row r="81" spans="1:5" ht="28.9" customHeight="1">
       <c r="A81" s="10" t="s">
         <v>149</v>
       </c>
@@ -5010,7 +5010,7 @@
       </c>
       <c r="E88" s="9"/>
     </row>
-    <row r="89" spans="1:5" ht="43.2" customHeight="1">
+    <row r="89" spans="1:5" ht="43.15" customHeight="1">
       <c r="A89" s="10" t="s">
         <v>149</v>
       </c>
@@ -5038,35 +5038,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AX10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="5" customWidth="1"/>
-    <col min="3" max="11" width="8.88671875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="6.88671875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.86328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" style="5" customWidth="1"/>
+    <col min="3" max="11" width="8.86328125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15.73046875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="6.86328125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="8.86328125" style="5" customWidth="1"/>
     <col min="15" max="15" width="12" style="5" customWidth="1"/>
-    <col min="16" max="17" width="8.88671875" style="5" customWidth="1"/>
-    <col min="18" max="18" width="16.109375" style="5" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" style="5" customWidth="1"/>
-    <col min="20" max="20" width="15.77734375" style="5" customWidth="1"/>
-    <col min="21" max="27" width="8.88671875" style="5" customWidth="1"/>
-    <col min="28" max="28" width="15.77734375" style="5" customWidth="1"/>
-    <col min="29" max="30" width="8.88671875" style="5" customWidth="1"/>
+    <col min="16" max="17" width="8.86328125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="16.1328125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="8.86328125" style="5" customWidth="1"/>
+    <col min="20" max="20" width="15.73046875" style="5" customWidth="1"/>
+    <col min="21" max="27" width="8.86328125" style="5" customWidth="1"/>
+    <col min="28" max="28" width="15.73046875" style="5" customWidth="1"/>
+    <col min="29" max="30" width="8.86328125" style="5" customWidth="1"/>
     <col min="31" max="31" width="12" style="5" customWidth="1"/>
-    <col min="32" max="35" width="8.88671875" style="5" customWidth="1"/>
-    <col min="36" max="36" width="16.77734375" style="5" customWidth="1"/>
-    <col min="37" max="44" width="8.88671875" style="5" customWidth="1"/>
-    <col min="45" max="46" width="9.88671875" style="5" customWidth="1"/>
-    <col min="47" max="47" width="9.109375" style="5" customWidth="1"/>
-    <col min="48" max="48" width="9.88671875" style="5" customWidth="1"/>
-    <col min="49" max="51" width="8.88671875" style="5" customWidth="1"/>
-    <col min="52" max="16384" width="8.88671875" style="5"/>
+    <col min="32" max="35" width="8.86328125" style="5" customWidth="1"/>
+    <col min="36" max="36" width="16.73046875" style="5" customWidth="1"/>
+    <col min="37" max="44" width="8.86328125" style="5" customWidth="1"/>
+    <col min="45" max="46" width="9.86328125" style="5" customWidth="1"/>
+    <col min="47" max="47" width="9.1328125" style="5" customWidth="1"/>
+    <col min="48" max="48" width="9.86328125" style="5" customWidth="1"/>
+    <col min="49" max="51" width="8.86328125" style="5" customWidth="1"/>
+    <col min="52" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="13.5" customHeight="1">
@@ -5232,17 +5232,17 @@
         <v>7</v>
       </c>
       <c r="D2" s="19">
-        <v>0.84</v>
+        <v>0.75</v>
       </c>
       <c r="E2" s="19">
-        <v>7.4999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F2" s="19" cm="1">
         <f t="array" ref="F2">D2/E2</f>
-        <v>11.2</v>
+        <v>10.714285714285714</v>
       </c>
       <c r="G2" s="19">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="H2" s="19">
         <v>7.0000000000000001E-3</v>
@@ -5257,7 +5257,7 @@
         <v>1</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="M2" s="21">
         <f>1/O2</f>
@@ -5271,7 +5271,7 @@
         <v>6</v>
       </c>
       <c r="P2" s="19">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="Q2" s="19">
         <v>0</v>
@@ -5283,20 +5283,20 @@
         <v>1.2</v>
       </c>
       <c r="T2" s="22" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="U2" s="19">
-        <v>0.1875</v>
+        <v>3.125E-2</v>
       </c>
       <c r="V2" s="19">
         <f t="shared" ref="V2" si="0">2*U2</f>
-        <v>0.375</v>
+        <v>6.25E-2</v>
       </c>
       <c r="W2" s="19">
         <v>4</v>
       </c>
       <c r="X2" s="19">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="Y2" s="19">
         <v>0</v>
@@ -5308,14 +5308,14 @@
         <v>1.2</v>
       </c>
       <c r="AB2" s="23" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="AC2" s="21">
-        <v>0.08</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AD2" s="19">
         <f t="shared" ref="AD2" si="1">2*AC2</f>
-        <v>0.16</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AE2" s="19">
         <v>2</v>
@@ -5333,7 +5333,7 @@
         <v>1.2</v>
       </c>
       <c r="AJ2" s="22" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="AK2" s="19">
         <v>0</v>
@@ -5808,24 +5808,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AY10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AY7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="5" customWidth="1"/>
-    <col min="3" max="42" width="8.88671875" style="5" customWidth="1"/>
-    <col min="43" max="43" width="11.88671875" style="5" customWidth="1"/>
-    <col min="44" max="44" width="8.88671875" style="5" customWidth="1"/>
-    <col min="45" max="45" width="9.88671875" style="5" customWidth="1"/>
-    <col min="46" max="46" width="10.109375" style="5" customWidth="1"/>
-    <col min="47" max="47" width="8.88671875" style="5" customWidth="1"/>
-    <col min="48" max="48" width="10.109375" style="5" customWidth="1"/>
-    <col min="49" max="49" width="11.88671875" style="5" customWidth="1"/>
-    <col min="50" max="52" width="8.88671875" style="5" customWidth="1"/>
-    <col min="53" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="8.86328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.86328125" style="5" customWidth="1"/>
+    <col min="3" max="42" width="8.86328125" style="5" customWidth="1"/>
+    <col min="43" max="43" width="11.86328125" style="5" customWidth="1"/>
+    <col min="44" max="44" width="8.86328125" style="5" customWidth="1"/>
+    <col min="45" max="45" width="9.86328125" style="5" customWidth="1"/>
+    <col min="46" max="46" width="10.1328125" style="5" customWidth="1"/>
+    <col min="47" max="47" width="8.86328125" style="5" customWidth="1"/>
+    <col min="48" max="48" width="10.1328125" style="5" customWidth="1"/>
+    <col min="49" max="49" width="11.86328125" style="5" customWidth="1"/>
+    <col min="50" max="52" width="8.86328125" style="5" customWidth="1"/>
+    <col min="53" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="14.1" customHeight="1">
@@ -5983,7 +5983,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="14.7" customHeight="1" thickBot="1">
+    <row r="2" spans="1:51" ht="14.65" customHeight="1" thickBot="1">
       <c r="A2" s="30" t="str" cm="1">
         <f t="array" ref="A2">Main_Input!A2</f>
         <v>Config1</v>
@@ -5998,119 +5998,119 @@
         <v>0.5</v>
       </c>
       <c r="E2" s="34">
-        <v>-0.54800000000000004</v>
+        <v>-0.36399999999999999</v>
       </c>
       <c r="F2" s="34">
-        <v>-0.438</v>
+        <v>-0.29199999999999998</v>
       </c>
       <c r="G2" s="34">
-        <v>-0.32900000000000001</v>
+        <v>-0.20799999999999999</v>
       </c>
       <c r="H2" s="34">
-        <v>-0.219</v>
+        <v>-0.122</v>
       </c>
       <c r="I2" s="34">
-        <v>-0.11</v>
+        <v>-4.7E-2</v>
       </c>
       <c r="J2" s="34">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="K2" s="34">
-        <v>0.11</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="L2" s="34">
-        <v>0.219</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="M2" s="34">
-        <v>0.32900000000000001</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="N2" s="34">
-        <v>0.438</v>
+        <v>0.318</v>
       </c>
       <c r="O2" s="34">
-        <v>0.54800000000000004</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="P2" s="34">
-        <v>0.65800000000000003</v>
+        <v>0.442</v>
       </c>
       <c r="Q2" s="34">
-        <v>0.76800000000000002</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="R2" s="34">
-        <v>0.877</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="S2" s="34">
-        <v>0.98699999999999999</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="T2" s="34">
-        <v>1.0960000000000001</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="U2" s="34">
-        <v>1.206</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="V2" s="34">
-        <v>1.3160000000000001</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="W2" s="35" cm="1">
         <f t="array" ref="W2">MAX(E2:V2)</f>
-        <v>1.3160000000000001</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="X2" s="34">
-        <v>4.4999999999999998E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="Y2" s="34">
-        <v>3.4000000000000002E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="Z2" s="34">
-        <v>2.5999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="AA2" s="34">
-        <v>0.02</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AB2" s="34">
-        <v>1.6E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="AC2" s="34">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="AD2" s="34">
-        <v>1.6E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AE2" s="34">
-        <v>2E-3</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AF2" s="34">
-        <v>2.5999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="AG2" s="34">
-        <v>3.4000000000000002E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AH2" s="34">
-        <v>4.4999999999999998E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AI2" s="34">
-        <v>5.8999999999999997E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="AJ2" s="34">
-        <v>7.3999999999999996E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="AK2" s="34">
-        <v>9.1999999999999998E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="AL2" s="34">
-        <v>0.113</v>
+        <v>0.105</v>
       </c>
       <c r="AM2" s="34">
-        <v>0.13600000000000001</v>
+        <v>0.154</v>
       </c>
       <c r="AN2" s="34">
-        <v>0.161</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="AO2" s="34">
-        <v>0.188</v>
+        <v>0.129</v>
       </c>
       <c r="AP2" s="36">
-        <v>1.4999999999999999E-2</v>
+        <v>154</v>
       </c>
       <c r="AQ2" s="31" t="s">
         <v>251</v>
@@ -6140,7 +6140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:51" ht="14.7" customHeight="1" thickBot="1">
+    <row r="3" spans="1:51" ht="14.65" customHeight="1" thickBot="1">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="32"/>
@@ -6193,7 +6193,7 @@
       <c r="AX3" s="32"/>
       <c r="AY3" s="32"/>
     </row>
-    <row r="4" spans="1:51" ht="14.7" customHeight="1" thickBot="1">
+    <row r="4" spans="1:51" ht="14.65" customHeight="1" thickBot="1">
       <c r="A4" s="30"/>
       <c r="B4" s="31"/>
       <c r="C4" s="32"/>
@@ -6246,7 +6246,7 @@
       <c r="AX4" s="32"/>
       <c r="AY4" s="32"/>
     </row>
-    <row r="5" spans="1:51" ht="14.7" customHeight="1" thickBot="1">
+    <row r="5" spans="1:51" ht="14.65" customHeight="1" thickBot="1">
       <c r="A5" s="30"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
@@ -6299,7 +6299,7 @@
       <c r="AX5" s="32"/>
       <c r="AY5" s="32"/>
     </row>
-    <row r="6" spans="1:51" ht="14.7" customHeight="1" thickBot="1">
+    <row r="6" spans="1:51" ht="14.65" customHeight="1" thickBot="1">
       <c r="A6" s="30"/>
       <c r="B6" s="31"/>
       <c r="C6" s="32"/>
@@ -6352,7 +6352,7 @@
       <c r="AX6" s="32"/>
       <c r="AY6" s="32"/>
     </row>
-    <row r="7" spans="1:51" ht="14.7" customHeight="1" thickBot="1">
+    <row r="7" spans="1:51" ht="14.65" customHeight="1" thickBot="1">
       <c r="A7" s="30"/>
       <c r="B7" s="31"/>
       <c r="C7" s="32"/>
@@ -6577,24 +6577,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="8.88671875" style="5" customWidth="1"/>
+    <col min="1" max="6" width="8.86328125" style="5" customWidth="1"/>
     <col min="7" max="7" width="10" style="5" customWidth="1"/>
-    <col min="8" max="18" width="8.88671875" style="5" customWidth="1"/>
-    <col min="19" max="20" width="10.109375" style="5" customWidth="1"/>
-    <col min="21" max="22" width="8.88671875" style="5" customWidth="1"/>
-    <col min="23" max="23" width="10.44140625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="5" customWidth="1"/>
-    <col min="25" max="25" width="8.88671875" style="5" customWidth="1"/>
-    <col min="26" max="16384" width="8.88671875" style="5"/>
+    <col min="8" max="18" width="8.86328125" style="5" customWidth="1"/>
+    <col min="19" max="20" width="10.1328125" style="5" customWidth="1"/>
+    <col min="21" max="22" width="8.86328125" style="5" customWidth="1"/>
+    <col min="23" max="23" width="10.3984375" style="5" customWidth="1"/>
+    <col min="24" max="24" width="9.86328125" style="5" customWidth="1"/>
+    <col min="25" max="25" width="8.86328125" style="5" customWidth="1"/>
+    <col min="26" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="14.4" customHeight="1">
+    <row r="1" spans="1:24" ht="14.45" customHeight="1">
       <c r="A1" s="37" t="s">
         <v>11</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="14.4" customHeight="1">
+    <row r="2" spans="1:24" ht="14.45" customHeight="1">
       <c r="A2" s="24" t="str" cm="1">
         <f t="array" ref="A2">Main_Input!A2</f>
         <v>Config1</v>
@@ -6728,22 +6728,22 @@
         <v>0</v>
       </c>
       <c r="T2" s="19">
-        <v>160</v>
+        <v>0.16</v>
       </c>
       <c r="U2" s="19">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="V2" s="19">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="W2" s="19">
-        <v>8.5000000000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="X2" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="14.4" customHeight="1">
+    <row r="3" spans="1:24" ht="14.45" customHeight="1">
       <c r="A3" s="24"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -6769,7 +6769,7 @@
       <c r="W3" s="24"/>
       <c r="X3" s="24"/>
     </row>
-    <row r="4" spans="1:24" ht="14.4" customHeight="1">
+    <row r="4" spans="1:24" ht="14.45" customHeight="1">
       <c r="A4" s="24"/>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
@@ -6795,7 +6795,7 @@
       <c r="W4" s="24"/>
       <c r="X4" s="24"/>
     </row>
-    <row r="5" spans="1:24" ht="14.4" customHeight="1">
+    <row r="5" spans="1:24" ht="14.45" customHeight="1">
       <c r="A5" s="24"/>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -6821,7 +6821,7 @@
       <c r="W5" s="24"/>
       <c r="X5" s="24"/>
     </row>
-    <row r="6" spans="1:24" ht="14.4" customHeight="1">
+    <row r="6" spans="1:24" ht="14.45" customHeight="1">
       <c r="A6" s="24"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -6847,7 +6847,7 @@
       <c r="W6" s="24"/>
       <c r="X6" s="24"/>
     </row>
-    <row r="7" spans="1:24" ht="14.4" customHeight="1">
+    <row r="7" spans="1:24" ht="14.45" customHeight="1">
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -6873,7 +6873,7 @@
       <c r="W7" s="24"/>
       <c r="X7" s="24"/>
     </row>
-    <row r="8" spans="1:24" ht="14.4" customHeight="1">
+    <row r="8" spans="1:24" ht="14.45" customHeight="1">
       <c r="A8" s="24"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
@@ -6899,7 +6899,7 @@
       <c r="W8" s="24"/>
       <c r="X8" s="24"/>
     </row>
-    <row r="9" spans="1:24" ht="14.4" customHeight="1">
+    <row r="9" spans="1:24" ht="14.45" customHeight="1">
       <c r="A9" s="24"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
@@ -6925,7 +6925,7 @@
       <c r="W9" s="24"/>
       <c r="X9" s="24"/>
     </row>
-    <row r="10" spans="1:24" ht="14.4" customHeight="1">
+    <row r="10" spans="1:24" ht="14.45" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
@@ -6951,7 +6951,7 @@
       <c r="W10" s="24"/>
       <c r="X10" s="24"/>
     </row>
-    <row r="11" spans="1:24" ht="14.4" customHeight="1">
+    <row r="11" spans="1:24" ht="14.45" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -6977,7 +6977,7 @@
       <c r="W11" s="24"/>
       <c r="X11" s="24"/>
     </row>
-    <row r="12" spans="1:24" ht="14.4" customHeight="1">
+    <row r="12" spans="1:24" ht="14.45" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
@@ -7003,7 +7003,7 @@
       <c r="W12" s="24"/>
       <c r="X12" s="24"/>
     </row>
-    <row r="13" spans="1:24" ht="14.4" customHeight="1">
+    <row r="13" spans="1:24" ht="14.45" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
@@ -7029,7 +7029,7 @@
       <c r="W13" s="24"/>
       <c r="X13" s="24"/>
     </row>
-    <row r="14" spans="1:24" ht="14.4" customHeight="1">
+    <row r="14" spans="1:24" ht="14.45" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
@@ -7055,7 +7055,7 @@
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
     </row>
-    <row r="15" spans="1:24" ht="14.4" customHeight="1">
+    <row r="15" spans="1:24" ht="14.45" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
@@ -7081,7 +7081,7 @@
       <c r="W15" s="24"/>
       <c r="X15" s="24"/>
     </row>
-    <row r="16" spans="1:24" ht="14.4" customHeight="1">
+    <row r="16" spans="1:24" ht="14.45" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
@@ -7107,7 +7107,7 @@
       <c r="W16" s="24"/>
       <c r="X16" s="24"/>
     </row>
-    <row r="17" spans="1:24" ht="14.4" customHeight="1">
+    <row r="17" spans="1:24" ht="14.45" customHeight="1">
       <c r="A17" s="24"/>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
@@ -7133,7 +7133,7 @@
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
     </row>
-    <row r="18" spans="1:24" ht="14.4" customHeight="1">
+    <row r="18" spans="1:24" ht="14.45" customHeight="1">
       <c r="A18" s="24"/>
       <c r="B18" s="24"/>
       <c r="C18" s="24"/>
@@ -7159,7 +7159,7 @@
       <c r="W18" s="24"/>
       <c r="X18" s="24"/>
     </row>
-    <row r="19" spans="1:24" ht="14.4" customHeight="1">
+    <row r="19" spans="1:24" ht="14.45" customHeight="1">
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
@@ -7185,7 +7185,7 @@
       <c r="W19" s="24"/>
       <c r="X19" s="24"/>
     </row>
-    <row r="20" spans="1:24" ht="14.4" customHeight="1">
+    <row r="20" spans="1:24" ht="14.45" customHeight="1">
       <c r="A20" s="24"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
@@ -7211,7 +7211,7 @@
       <c r="W20" s="24"/>
       <c r="X20" s="24"/>
     </row>
-    <row r="21" spans="1:24" ht="14.4" customHeight="1">
+    <row r="21" spans="1:24" ht="14.45" customHeight="1">
       <c r="A21" s="39"/>
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
@@ -7237,7 +7237,7 @@
       <c r="W21" s="40"/>
       <c r="X21" s="41"/>
     </row>
-    <row r="22" spans="1:24" ht="14.4" customHeight="1">
+    <row r="22" spans="1:24" ht="14.45" customHeight="1">
       <c r="A22" s="42"/>
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
@@ -7263,7 +7263,7 @@
       <c r="W22" s="42"/>
       <c r="X22" s="42"/>
     </row>
-    <row r="23" spans="1:24" ht="14.4" customHeight="1">
+    <row r="23" spans="1:24" ht="14.45" customHeight="1">
       <c r="A23" s="43"/>
       <c r="B23" s="43"/>
       <c r="C23" s="43"/>
@@ -7289,7 +7289,7 @@
       <c r="W23" s="43"/>
       <c r="X23" s="43"/>
     </row>
-    <row r="24" spans="1:24" ht="14.4" customHeight="1">
+    <row r="24" spans="1:24" ht="14.45" customHeight="1">
       <c r="A24" s="43"/>
       <c r="B24" s="43"/>
       <c r="C24" s="43"/>
@@ -7315,7 +7315,7 @@
       <c r="W24" s="43"/>
       <c r="X24" s="43"/>
     </row>
-    <row r="25" spans="1:24" ht="14.4" customHeight="1">
+    <row r="25" spans="1:24" ht="14.45" customHeight="1">
       <c r="A25" s="43"/>
       <c r="B25" s="43"/>
       <c r="C25" s="43"/>
@@ -7341,7 +7341,7 @@
       <c r="W25" s="43"/>
       <c r="X25" s="43"/>
     </row>
-    <row r="26" spans="1:24" ht="14.4" customHeight="1">
+    <row r="26" spans="1:24" ht="14.45" customHeight="1">
       <c r="A26" s="43"/>
       <c r="B26" s="43"/>
       <c r="C26" s="43"/>
@@ -7367,7 +7367,7 @@
       <c r="W26" s="43"/>
       <c r="X26" s="43"/>
     </row>
-    <row r="27" spans="1:24" ht="14.4" customHeight="1">
+    <row r="27" spans="1:24" ht="14.45" customHeight="1">
       <c r="A27" s="43"/>
       <c r="B27" s="43"/>
       <c r="C27" s="43"/>
@@ -7393,7 +7393,7 @@
       <c r="W27" s="43"/>
       <c r="X27" s="43"/>
     </row>
-    <row r="28" spans="1:24" ht="14.4" customHeight="1">
+    <row r="28" spans="1:24" ht="14.45" customHeight="1">
       <c r="A28" s="43"/>
       <c r="B28" s="43"/>
       <c r="C28" s="43"/>
@@ -7419,7 +7419,7 @@
       <c r="W28" s="43"/>
       <c r="X28" s="43"/>
     </row>
-    <row r="29" spans="1:24" ht="14.4" customHeight="1">
+    <row r="29" spans="1:24" ht="14.45" customHeight="1">
       <c r="A29" s="43"/>
       <c r="B29" s="43"/>
       <c r="C29" s="43"/>
@@ -7445,7 +7445,7 @@
       <c r="W29" s="43"/>
       <c r="X29" s="43"/>
     </row>
-    <row r="30" spans="1:24" ht="14.4" customHeight="1">
+    <row r="30" spans="1:24" ht="14.45" customHeight="1">
       <c r="A30" s="43"/>
       <c r="B30" s="43"/>
       <c r="C30" s="43"/>
@@ -7471,7 +7471,7 @@
       <c r="W30" s="43"/>
       <c r="X30" s="43"/>
     </row>
-    <row r="31" spans="1:24" ht="14.4" customHeight="1">
+    <row r="31" spans="1:24" ht="14.45" customHeight="1">
       <c r="A31" s="43"/>
       <c r="B31" s="43"/>
       <c r="C31" s="43"/>
@@ -7497,7 +7497,7 @@
       <c r="W31" s="43"/>
       <c r="X31" s="43"/>
     </row>
-    <row r="32" spans="1:24" ht="14.4" customHeight="1">
+    <row r="32" spans="1:24" ht="14.45" customHeight="1">
       <c r="A32" s="43"/>
       <c r="B32" s="43"/>
       <c r="C32" s="43"/>
@@ -7523,7 +7523,7 @@
       <c r="W32" s="43"/>
       <c r="X32" s="43"/>
     </row>
-    <row r="33" spans="1:24" ht="14.4" customHeight="1">
+    <row r="33" spans="1:24" ht="14.45" customHeight="1">
       <c r="A33" s="43"/>
       <c r="B33" s="43"/>
       <c r="C33" s="43"/>
@@ -7549,7 +7549,7 @@
       <c r="W33" s="43"/>
       <c r="X33" s="43"/>
     </row>
-    <row r="34" spans="1:24" ht="14.4" customHeight="1">
+    <row r="34" spans="1:24" ht="14.45" customHeight="1">
       <c r="A34" s="43"/>
       <c r="B34" s="43"/>
       <c r="C34" s="43"/>
@@ -7575,7 +7575,7 @@
       <c r="W34" s="43"/>
       <c r="X34" s="43"/>
     </row>
-    <row r="35" spans="1:24" ht="14.4" customHeight="1">
+    <row r="35" spans="1:24" ht="14.45" customHeight="1">
       <c r="A35" s="43"/>
       <c r="B35" s="43"/>
       <c r="C35" s="43"/>
@@ -7601,7 +7601,7 @@
       <c r="W35" s="43"/>
       <c r="X35" s="43"/>
     </row>
-    <row r="36" spans="1:24" ht="14.4" customHeight="1">
+    <row r="36" spans="1:24" ht="14.45" customHeight="1">
       <c r="A36" s="43"/>
       <c r="B36" s="43"/>
       <c r="C36" s="43"/>
@@ -7627,7 +7627,7 @@
       <c r="W36" s="43"/>
       <c r="X36" s="43"/>
     </row>
-    <row r="37" spans="1:24" ht="14.4" customHeight="1">
+    <row r="37" spans="1:24" ht="14.45" customHeight="1">
       <c r="A37" s="43"/>
       <c r="B37" s="43"/>
       <c r="C37" s="43"/>
@@ -7653,7 +7653,7 @@
       <c r="W37" s="43"/>
       <c r="X37" s="43"/>
     </row>
-    <row r="38" spans="1:24" ht="14.4" customHeight="1">
+    <row r="38" spans="1:24" ht="14.45" customHeight="1">
       <c r="A38" s="43"/>
       <c r="B38" s="43"/>
       <c r="C38" s="43"/>
@@ -7679,7 +7679,7 @@
       <c r="W38" s="43"/>
       <c r="X38" s="43"/>
     </row>
-    <row r="39" spans="1:24" ht="14.4" customHeight="1">
+    <row r="39" spans="1:24" ht="14.45" customHeight="1">
       <c r="A39" s="43"/>
       <c r="B39" s="43"/>
       <c r="C39" s="43"/>
@@ -7705,7 +7705,7 @@
       <c r="W39" s="43"/>
       <c r="X39" s="43"/>
     </row>
-    <row r="40" spans="1:24" ht="14.4" customHeight="1">
+    <row r="40" spans="1:24" ht="14.45" customHeight="1">
       <c r="A40" s="43"/>
       <c r="B40" s="43"/>
       <c r="C40" s="43"/>
@@ -7731,7 +7731,7 @@
       <c r="W40" s="43"/>
       <c r="X40" s="43"/>
     </row>
-    <row r="41" spans="1:24" ht="14.4" customHeight="1">
+    <row r="41" spans="1:24" ht="14.45" customHeight="1">
       <c r="A41" s="43"/>
       <c r="B41" s="43"/>
       <c r="C41" s="43"/>
@@ -7757,7 +7757,7 @@
       <c r="W41" s="43"/>
       <c r="X41" s="43"/>
     </row>
-    <row r="42" spans="1:24" ht="14.4" customHeight="1">
+    <row r="42" spans="1:24" ht="14.45" customHeight="1">
       <c r="A42" s="43"/>
       <c r="B42" s="43"/>
       <c r="C42" s="43"/>
@@ -7783,7 +7783,7 @@
       <c r="W42" s="43"/>
       <c r="X42" s="43"/>
     </row>
-    <row r="43" spans="1:24" ht="14.4" customHeight="1">
+    <row r="43" spans="1:24" ht="14.45" customHeight="1">
       <c r="A43" s="43"/>
       <c r="B43" s="43"/>
       <c r="C43" s="43"/>
@@ -7809,7 +7809,7 @@
       <c r="W43" s="43"/>
       <c r="X43" s="43"/>
     </row>
-    <row r="44" spans="1:24" ht="14.4" customHeight="1">
+    <row r="44" spans="1:24" ht="14.45" customHeight="1">
       <c r="A44" s="43"/>
       <c r="B44" s="43"/>
       <c r="C44" s="43"/>
@@ -7835,7 +7835,7 @@
       <c r="W44" s="43"/>
       <c r="X44" s="43"/>
     </row>
-    <row r="45" spans="1:24" ht="14.4" customHeight="1">
+    <row r="45" spans="1:24" ht="14.45" customHeight="1">
       <c r="A45" s="43"/>
       <c r="B45" s="43"/>
       <c r="C45" s="43"/>
@@ -7861,7 +7861,7 @@
       <c r="W45" s="43"/>
       <c r="X45" s="43"/>
     </row>
-    <row r="46" spans="1:24" ht="14.4" customHeight="1">
+    <row r="46" spans="1:24" ht="14.45" customHeight="1">
       <c r="A46" s="43"/>
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
@@ -7887,7 +7887,7 @@
       <c r="W46" s="43"/>
       <c r="X46" s="43"/>
     </row>
-    <row r="47" spans="1:24" ht="14.4" customHeight="1">
+    <row r="47" spans="1:24" ht="14.45" customHeight="1">
       <c r="A47" s="43"/>
       <c r="B47" s="43"/>
       <c r="C47" s="43"/>
@@ -7913,7 +7913,7 @@
       <c r="W47" s="43"/>
       <c r="X47" s="43"/>
     </row>
-    <row r="48" spans="1:24" ht="14.4" customHeight="1">
+    <row r="48" spans="1:24" ht="14.45" customHeight="1">
       <c r="A48" s="43"/>
       <c r="B48" s="43"/>
       <c r="C48" s="43"/>
@@ -7939,7 +7939,7 @@
       <c r="W48" s="43"/>
       <c r="X48" s="43"/>
     </row>
-    <row r="49" spans="1:24" ht="14.4" customHeight="1">
+    <row r="49" spans="1:24" ht="14.45" customHeight="1">
       <c r="A49" s="43"/>
       <c r="B49" s="43"/>
       <c r="C49" s="43"/>
@@ -7965,7 +7965,7 @@
       <c r="W49" s="43"/>
       <c r="X49" s="43"/>
     </row>
-    <row r="50" spans="1:24" ht="14.4" customHeight="1">
+    <row r="50" spans="1:24" ht="14.45" customHeight="1">
       <c r="A50" s="43"/>
       <c r="B50" s="43"/>
       <c r="C50" s="43"/>
@@ -7991,7 +7991,7 @@
       <c r="W50" s="43"/>
       <c r="X50" s="43"/>
     </row>
-    <row r="51" spans="1:24" ht="14.4" customHeight="1">
+    <row r="51" spans="1:24" ht="14.45" customHeight="1">
       <c r="A51" s="43"/>
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
@@ -8017,7 +8017,7 @@
       <c r="W51" s="43"/>
       <c r="X51" s="43"/>
     </row>
-    <row r="52" spans="1:24" ht="14.4" customHeight="1">
+    <row r="52" spans="1:24" ht="14.45" customHeight="1">
       <c r="A52" s="43"/>
       <c r="B52" s="43"/>
       <c r="C52" s="43"/>
@@ -8043,7 +8043,7 @@
       <c r="W52" s="43"/>
       <c r="X52" s="43"/>
     </row>
-    <row r="53" spans="1:24" ht="14.4" customHeight="1">
+    <row r="53" spans="1:24" ht="14.45" customHeight="1">
       <c r="A53" s="43"/>
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
@@ -8069,7 +8069,7 @@
       <c r="W53" s="43"/>
       <c r="X53" s="43"/>
     </row>
-    <row r="54" spans="1:24" ht="14.4" customHeight="1">
+    <row r="54" spans="1:24" ht="14.45" customHeight="1">
       <c r="A54" s="43"/>
       <c r="B54" s="43"/>
       <c r="C54" s="43"/>
@@ -8095,7 +8095,7 @@
       <c r="W54" s="43"/>
       <c r="X54" s="43"/>
     </row>
-    <row r="55" spans="1:24" ht="14.4" customHeight="1">
+    <row r="55" spans="1:24" ht="14.45" customHeight="1">
       <c r="A55" s="43"/>
       <c r="B55" s="43"/>
       <c r="C55" s="43"/>
@@ -8121,7 +8121,7 @@
       <c r="W55" s="43"/>
       <c r="X55" s="43"/>
     </row>
-    <row r="56" spans="1:24" ht="14.4" customHeight="1">
+    <row r="56" spans="1:24" ht="14.45" customHeight="1">
       <c r="A56" s="43"/>
       <c r="B56" s="43"/>
       <c r="C56" s="43"/>
@@ -8162,20 +8162,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" style="5" customWidth="1"/>
-    <col min="6" max="8" width="14.109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="13.1328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.265625" style="5" customWidth="1"/>
+    <col min="6" max="8" width="14.1328125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.86328125" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13.5" customHeight="1">
@@ -8342,10 +8340,10 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="24" width="8.88671875" style="5" customWidth="1"/>
-    <col min="25" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="24" width="8.86328125" style="5" customWidth="1"/>
+    <col min="25" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
@@ -8937,7 +8935,7 @@
       <c r="V19" s="50"/>
       <c r="W19" s="50"/>
     </row>
-    <row r="20" spans="1:23" ht="14.4" customHeight="1">
+    <row r="20" spans="1:23" ht="14.45" customHeight="1">
       <c r="A20" s="54"/>
       <c r="B20" s="54"/>
       <c r="C20" s="54"/>
@@ -8962,7 +8960,7 @@
       <c r="V20" s="50"/>
       <c r="W20" s="50"/>
     </row>
-    <row r="21" spans="1:23" ht="14.4" customHeight="1">
+    <row r="21" spans="1:23" ht="14.45" customHeight="1">
       <c r="A21" s="50"/>
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
@@ -9003,7 +9001,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.9" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
   </cols>

</xml_diff>